<commit_message>
copy excel file - trying to copy formatting as well
</commit_message>
<xml_diff>
--- a/genai/text2.xlsx
+++ b/genai/text2.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Source\Repos\learning\genai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1752A5BA-E09C-4575-B1BB-E14CD13DB8F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE3C90C-3553-4983-8A6F-4195C3D4B27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Translated_Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>hun</t>
   </si>
@@ -34,35 +33,18 @@
   <si>
     <t>Államháztartási hiány GDP arányosan</t>
   </si>
-  <si>
-    <t>translated_hun</t>
-  </si>
-  <si>
-    <t>['God bless the seed.']</t>
-  </si>
-  <si>
-    <t>["It's only the Fidesz."]</t>
-  </si>
-  <si>
-    <t>['State deficit in proportion to GDP']</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Aptos Narrow"/>
     </font>
   </fonts>
   <fills count="2">
@@ -73,7 +55,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -81,30 +63,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,55 +437,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="31.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.36328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>